<commit_message>
back slash issue for mac
</commit_message>
<xml_diff>
--- a/BIS232_SCRIPT_EXCLUSION_REQUEST/input_data/datapool/EXCLUSION_REQUEST.xlsx
+++ b/BIS232_SCRIPT_EXCLUSION_REQUEST/input_data/datapool/EXCLUSION_REQUEST.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2842CFCE-9590-496C-B16E-FDD8EAD35330}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F79D134-0D74-4EE3-A8E0-B63FBA75F2CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1056" windowWidth="19008" windowHeight="7920" tabRatio="582" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1056" windowWidth="19008" windowHeight="7920" tabRatio="582" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="14" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Step 3" sheetId="1" r:id="rId4"/>
     <sheet name="Step 4" sheetId="12" r:id="rId5"/>
     <sheet name="Step 5" sheetId="11" r:id="rId6"/>
-    <sheet name="dropdowns" sheetId="7" r:id="rId7"/>
+    <sheet name="dropdowns" sheetId="7" state="hidden" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="activity">dropdowns!$F$1:$F$6</definedName>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="579">
   <si>
     <t>Active</t>
   </si>
@@ -287,12 +287,6 @@
     <t>12|41</t>
   </si>
   <si>
-    <t>12|-33</t>
-  </si>
-  <si>
-    <t>-12.5|-3.6</t>
-  </si>
-  <si>
     <t>0|35</t>
   </si>
   <si>
@@ -317,9 +311,6 @@
     <t>4.4|43</t>
   </si>
   <si>
-    <t>-12|</t>
-  </si>
-  <si>
     <t>|344</t>
   </si>
   <si>
@@ -686,9 +677,6 @@
     <t>HTSUS Code</t>
   </si>
   <si>
-    <t>343</t>
-  </si>
-  <si>
     <t>Authorized Representative Phone Number</t>
   </si>
   <si>
@@ -1742,12 +1730,6 @@
     <t>Scenario_05</t>
   </si>
   <si>
-    <t>7216500000</t>
-  </si>
-  <si>
-    <t>7606923030</t>
-  </si>
-  <si>
     <t>2235 pimmit</t>
   </si>
   <si>
@@ -1779,6 +1761,36 @@
   </si>
   <si>
     <t>23232dd</t>
+  </si>
+  <si>
+    <t>12.5|3.6</t>
+  </si>
+  <si>
+    <t>12|</t>
+  </si>
+  <si>
+    <t>99|11</t>
+  </si>
+  <si>
+    <t>0|41</t>
+  </si>
+  <si>
+    <t>7208103000</t>
+  </si>
+  <si>
+    <t>adress</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Exclusion Quantity</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -1979,7 +1991,7 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="102">
+  <dxfs count="104">
     <dxf>
       <font>
         <strike val="0"/>
@@ -2294,6 +2306,12 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2766,31 +2784,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6B50D941-9E7D-49EF-85D4-20B0C5C539E4}" name="Table5" displayName="Table5" ref="B1:W6" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6B50D941-9E7D-49EF-85D4-20B0C5C539E4}" name="Table5" displayName="Table5" ref="B1:W6" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
   <autoFilter ref="B1:W6" xr:uid="{9ECCDE69-E40D-4163-B6A5-E6B3FB52F5C0}"/>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{874E953C-DFF0-4F8C-842D-CAF927DC06DA}" name="Metal Type" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{7F0046B2-7149-432A-974A-7E6E8646791B}" name="Metal Class" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{69C3ADD4-C00B-48F7-AF9F-3E944C3009C8}" name="HTSUS Code" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{CBDB2A5E-5C0B-47F6-A799-AE378374FC02}" name="Organization Legal Name" dataDxfId="96"/>
-    <tableColumn id="5" xr3:uid="{AF628F9B-244E-43AD-BBEC-C5D23C81AD8D}" name="Requesting Organization Street Address" dataDxfId="95"/>
-    <tableColumn id="6" xr3:uid="{E331060B-B473-452C-BB4C-2F2A0AAB73AC}" name="Requesting Organization City" dataDxfId="94"/>
-    <tableColumn id="7" xr3:uid="{0276E142-D728-4A90-8644-0CA4FAF86156}" name="Requesting Organization State" dataDxfId="93"/>
-    <tableColumn id="8" xr3:uid="{F684105D-A196-4959-A40B-1ED160A291AB}" name="Requesting Organization Zipcode" dataDxfId="92"/>
-    <tableColumn id="9" xr3:uid="{E9E1439C-F013-4849-A83B-BC6E7455FED4}" name="Requesting Organization POC Name" dataDxfId="91"/>
-    <tableColumn id="10" xr3:uid="{C74C9FDD-8E8B-4B0F-B07F-2E312DCCBB33}" name="Requesting Organization Phone Number" dataDxfId="90"/>
-    <tableColumn id="11" xr3:uid="{FBF8D0FE-5C12-495C-810A-CD20D4100D29}" name="Requesting Organization Email Address" dataDxfId="89"/>
-    <tableColumn id="12" xr3:uid="{F76750BC-C735-45CD-8149-F05A653206D5}" name="Requesting Organization Website Address" dataDxfId="88"/>
-    <tableColumn id="13" xr3:uid="{27F303FB-99DC-4DD1-A3FB-0ED1D2C97DB7}" name="Importer Legal Name" dataDxfId="87"/>
-    <tableColumn id="14" xr3:uid="{77FDE049-15A5-4864-B272-347EFF413CA5}" name="Importer Street Address" dataDxfId="86"/>
-    <tableColumn id="15" xr3:uid="{23F58BAC-C5F5-4475-8805-45565C87B0A8}" name="Importer City" dataDxfId="85"/>
-    <tableColumn id="16" xr3:uid="{89C47DDF-7378-4505-9713-43DA16C9F95D}" name="Importer State" dataDxfId="84"/>
-    <tableColumn id="17" xr3:uid="{940B9F02-16BB-4C64-AE98-337E9D757CE5}" name="Importer Zipcode" dataDxfId="83"/>
-    <tableColumn id="18" xr3:uid="{EECE9370-AA28-4DCD-9FF4-08A3B6C1032D}" name="Importer POC Name" dataDxfId="82"/>
-    <tableColumn id="19" xr3:uid="{E903BCBC-25C2-4DDE-A73C-0AE7AFBF649E}" name="Importer Phone Number" dataDxfId="81"/>
-    <tableColumn id="20" xr3:uid="{0CFB9ADB-35F9-413D-8C7E-072786A828BD}" name="Importer Email Address" dataDxfId="80"/>
-    <tableColumn id="21" xr3:uid="{5B4F4E14-F9DF-4791-BD6B-53E1E4CAB301}" name="Importer Website Address" dataDxfId="79"/>
-    <tableColumn id="22" xr3:uid="{F8C0F930-DAAE-4BEB-AEE4-7CCE3D66602B}" name="Active" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{874E953C-DFF0-4F8C-842D-CAF927DC06DA}" name="Metal Type" dataDxfId="101"/>
+    <tableColumn id="2" xr3:uid="{7F0046B2-7149-432A-974A-7E6E8646791B}" name="Metal Class" dataDxfId="100"/>
+    <tableColumn id="3" xr3:uid="{69C3ADD4-C00B-48F7-AF9F-3E944C3009C8}" name="HTSUS Code" dataDxfId="99"/>
+    <tableColumn id="4" xr3:uid="{CBDB2A5E-5C0B-47F6-A799-AE378374FC02}" name="Organization Legal Name" dataDxfId="98"/>
+    <tableColumn id="5" xr3:uid="{AF628F9B-244E-43AD-BBEC-C5D23C81AD8D}" name="Requesting Organization Street Address" dataDxfId="97"/>
+    <tableColumn id="6" xr3:uid="{E331060B-B473-452C-BB4C-2F2A0AAB73AC}" name="Requesting Organization City" dataDxfId="96"/>
+    <tableColumn id="7" xr3:uid="{0276E142-D728-4A90-8644-0CA4FAF86156}" name="Requesting Organization State" dataDxfId="95"/>
+    <tableColumn id="8" xr3:uid="{F684105D-A196-4959-A40B-1ED160A291AB}" name="Requesting Organization Zipcode" dataDxfId="94"/>
+    <tableColumn id="9" xr3:uid="{E9E1439C-F013-4849-A83B-BC6E7455FED4}" name="Requesting Organization POC Name" dataDxfId="93"/>
+    <tableColumn id="10" xr3:uid="{C74C9FDD-8E8B-4B0F-B07F-2E312DCCBB33}" name="Requesting Organization Phone Number" dataDxfId="92"/>
+    <tableColumn id="11" xr3:uid="{FBF8D0FE-5C12-495C-810A-CD20D4100D29}" name="Requesting Organization Email Address" dataDxfId="91"/>
+    <tableColumn id="12" xr3:uid="{F76750BC-C735-45CD-8149-F05A653206D5}" name="Requesting Organization Website Address" dataDxfId="90"/>
+    <tableColumn id="13" xr3:uid="{27F303FB-99DC-4DD1-A3FB-0ED1D2C97DB7}" name="Importer Legal Name" dataDxfId="89"/>
+    <tableColumn id="14" xr3:uid="{77FDE049-15A5-4864-B272-347EFF413CA5}" name="Importer Street Address" dataDxfId="88"/>
+    <tableColumn id="15" xr3:uid="{23F58BAC-C5F5-4475-8805-45565C87B0A8}" name="Importer City" dataDxfId="87"/>
+    <tableColumn id="16" xr3:uid="{89C47DDF-7378-4505-9713-43DA16C9F95D}" name="Importer State" dataDxfId="86"/>
+    <tableColumn id="17" xr3:uid="{940B9F02-16BB-4C64-AE98-337E9D757CE5}" name="Importer Zipcode" dataDxfId="85"/>
+    <tableColumn id="18" xr3:uid="{EECE9370-AA28-4DCD-9FF4-08A3B6C1032D}" name="Importer POC Name" dataDxfId="84"/>
+    <tableColumn id="19" xr3:uid="{E903BCBC-25C2-4DDE-A73C-0AE7AFBF649E}" name="Importer Phone Number" dataDxfId="83"/>
+    <tableColumn id="20" xr3:uid="{0CFB9ADB-35F9-413D-8C7E-072786A828BD}" name="Importer Email Address" dataDxfId="82"/>
+    <tableColumn id="21" xr3:uid="{5B4F4E14-F9DF-4791-BD6B-53E1E4CAB301}" name="Importer Website Address" dataDxfId="81"/>
+    <tableColumn id="22" xr3:uid="{F8C0F930-DAAE-4BEB-AEE4-7CCE3D66602B}" name="Active" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2800,22 +2818,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C00CC6D0-AED8-4B50-8440-B7C10D6C50B7}" name="Table4" displayName="Table4" ref="B1:R5" totalsRowShown="0">
   <autoFilter ref="B1:R5" xr:uid="{BEF2A08F-EC42-4EA3-B95F-EC8C3A015570}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{0FA206D9-DC3A-49C5-80DA-A98EE3AB2425}" name="Authorized Representative Phone Number" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{123D9AA7-0D9A-4E89-B688-3DF79AD83AFC}" name="Authorized Representative Email Address" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{0038E7FC-EDE4-43F2-83F6-E202B2DC0503}" name="Authorized Representative Website Address" dataDxfId="75"/>
-    <tableColumn id="4" xr3:uid="{15583359-F896-42FA-A1A7-0284EC940134}" name="Ownership Activity" dataDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{E5E39915-5300-423B-843C-B4ACF34B9998}" name="Ownership Organization Name" dataDxfId="73"/>
-    <tableColumn id="6" xr3:uid="{1F367CA3-1C24-48F9-B123-75F10D990769}" name="Ownership Headquarters Country" dataDxfId="72"/>
-    <tableColumn id="7" xr3:uid="{BB865DF0-8C20-477B-A377-26ACED1127C6}" name="Total Requested Annual Exclusion Quantity" dataDxfId="71"/>
-    <tableColumn id="8" xr3:uid="{D3A4B3A5-AD12-4F6C-85A4-78099AC137DF}" name="Total Requested Average Annual Consumption" dataDxfId="70"/>
-    <tableColumn id="9" xr3:uid="{6B93A08D-952A-4712-AF29-63A359295021}" name="Exclusion Explanation" dataDxfId="69"/>
-    <tableColumn id="10" xr3:uid="{E771DDAE-EBF8-4591-9E99-AC1AFE87498E}" name="Percentage Not Available" dataDxfId="68"/>
-    <tableColumn id="11" xr3:uid="{B1B25C5C-120C-44E2-B09E-97263F7D33E2}" name="Delivery Estimate" dataDxfId="67"/>
-    <tableColumn id="12" xr3:uid="{6AD62AFD-4B80-40AE-83D8-21056F452A02}" name="Manufacture Estimate" dataDxfId="66"/>
-    <tableColumn id="13" xr3:uid="{83B2B849-F333-4FF1-8872-6A1DDA3B050A}" name="Shipment Days Estimate" dataDxfId="65"/>
-    <tableColumn id="14" xr3:uid="{7DA19601-DBE8-4EC3-88D0-AB8C18295D87}" name="Shipment Quantity Estimate" dataDxfId="64"/>
-    <tableColumn id="15" xr3:uid="{128AEB11-8FA3-4A8C-94D8-EA71D67C6106}" name="Non US Producer Name" dataDxfId="63"/>
-    <tableColumn id="16" xr3:uid="{32AA5005-53F1-4B52-B376-EE7E70108241}" name="Non US Producer Headquarters Country" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{0FA206D9-DC3A-49C5-80DA-A98EE3AB2425}" name="Authorized Representative Phone Number" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{123D9AA7-0D9A-4E89-B688-3DF79AD83AFC}" name="Authorized Representative Email Address" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{0038E7FC-EDE4-43F2-83F6-E202B2DC0503}" name="Authorized Representative Website Address" dataDxfId="77"/>
+    <tableColumn id="4" xr3:uid="{15583359-F896-42FA-A1A7-0284EC940134}" name="Ownership Activity" dataDxfId="76"/>
+    <tableColumn id="5" xr3:uid="{E5E39915-5300-423B-843C-B4ACF34B9998}" name="Ownership Organization Name" dataDxfId="75"/>
+    <tableColumn id="6" xr3:uid="{1F367CA3-1C24-48F9-B123-75F10D990769}" name="Ownership Headquarters Country" dataDxfId="74"/>
+    <tableColumn id="7" xr3:uid="{BB865DF0-8C20-477B-A377-26ACED1127C6}" name="Total Requested Annual Exclusion Quantity" dataDxfId="73"/>
+    <tableColumn id="8" xr3:uid="{D3A4B3A5-AD12-4F6C-85A4-78099AC137DF}" name="Total Requested Average Annual Consumption" dataDxfId="72"/>
+    <tableColumn id="9" xr3:uid="{6B93A08D-952A-4712-AF29-63A359295021}" name="Exclusion Explanation" dataDxfId="71"/>
+    <tableColumn id="10" xr3:uid="{E771DDAE-EBF8-4591-9E99-AC1AFE87498E}" name="Percentage Not Available" dataDxfId="70"/>
+    <tableColumn id="11" xr3:uid="{B1B25C5C-120C-44E2-B09E-97263F7D33E2}" name="Delivery Estimate" dataDxfId="69"/>
+    <tableColumn id="12" xr3:uid="{6AD62AFD-4B80-40AE-83D8-21056F452A02}" name="Manufacture Estimate" dataDxfId="68"/>
+    <tableColumn id="13" xr3:uid="{83B2B849-F333-4FF1-8872-6A1DDA3B050A}" name="Shipment Days Estimate" dataDxfId="67"/>
+    <tableColumn id="14" xr3:uid="{7DA19601-DBE8-4EC3-88D0-AB8C18295D87}" name="Shipment Quantity Estimate" dataDxfId="66"/>
+    <tableColumn id="15" xr3:uid="{128AEB11-8FA3-4A8C-94D8-EA71D67C6106}" name="Non US Producer Name" dataDxfId="65"/>
+    <tableColumn id="16" xr3:uid="{32AA5005-53F1-4B52-B376-EE7E70108241}" name="Non US Producer Headquarters Country" dataDxfId="64"/>
     <tableColumn id="17" xr3:uid="{A9BF9B11-8DBE-4789-9BD1-4879D8D39A77}" name="Active"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2823,53 +2841,53 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18837768-C9F7-4E2E-A234-3C49EE851E42}" name="Table1" displayName="Table1" ref="B1:AU5" totalsRowShown="0" headerRowDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18837768-C9F7-4E2E-A234-3C49EE851E42}" name="Table1" displayName="Table1" ref="B1:AU6" totalsRowShown="0" headerRowDxfId="63">
   <tableColumns count="46">
-    <tableColumn id="52" xr3:uid="{AF00D49C-0A7D-4826-8506-CA4526F98C11}" name="Product Description" dataDxfId="60" dataCellStyle="Neutral"/>
-    <tableColumn id="2" xr3:uid="{A687C822-C58F-452D-B26B-CD9856126779}" name="Aluminum" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{B1E51DF4-E370-4B45-B934-CA4680543E00}" name="Antimony" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{7D4E5A00-87A1-4DB6-9285-237214866EA7}" name="Bismuth" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{FF6AE917-6EF7-453D-B900-491D429EA10B}" name="Boron" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{C6ABA99D-1825-4988-8F10-DA21B5E30466}" name="Carbon" dataDxfId="55"/>
-    <tableColumn id="7" xr3:uid="{91DDBD07-BA6D-41D3-9082-B8FF3D52C3E3}" name="Chromium" dataDxfId="54"/>
-    <tableColumn id="8" xr3:uid="{BA93B31C-68BB-4929-94DC-EAD966AE376B}" name="Cobalt" dataDxfId="53"/>
-    <tableColumn id="9" xr3:uid="{1FDAC7B7-2C23-4E6E-92BF-72B3374222D5}" name="Copper" dataDxfId="52"/>
-    <tableColumn id="10" xr3:uid="{27E624C3-C609-4CA7-8BE0-5CE724DAB152}" name="Iron" dataDxfId="51"/>
-    <tableColumn id="11" xr3:uid="{7DBD8888-7842-48EA-AE28-BEE69CF5DC79}" name="Lead" dataDxfId="50"/>
-    <tableColumn id="28" xr3:uid="{DF0716E0-9874-4A86-8764-FB0155320B9F}" name="Magnesium" dataDxfId="49"/>
-    <tableColumn id="12" xr3:uid="{F4F409FB-A7C8-4EB9-8DCC-EE00D05071BC}" name="Manganese" dataDxfId="48"/>
-    <tableColumn id="13" xr3:uid="{DEA2DC2F-313C-4BC9-8D50-5353297D4F05}" name="Molybdenum" dataDxfId="47"/>
-    <tableColumn id="14" xr3:uid="{43C014BD-631A-4A5B-A695-5EE01DBB3143}" name="Nickel" dataDxfId="46"/>
-    <tableColumn id="15" xr3:uid="{2D60D17D-1D84-4C39-8B26-9695D79B6202}" name="Niobium" dataDxfId="45"/>
-    <tableColumn id="16" xr3:uid="{31EFBEBA-E25A-414C-9C97-44B44C2668F7}" name="Nitrogen" dataDxfId="44"/>
-    <tableColumn id="17" xr3:uid="{67D70C10-B973-4F94-9919-EEE95AABDDE6}" name="Phosphorus" dataDxfId="43"/>
-    <tableColumn id="18" xr3:uid="{6966F273-C0D5-4B0D-B67C-96CA2143F39B}" name="Selenium" dataDxfId="42"/>
-    <tableColumn id="19" xr3:uid="{34637CE8-6F73-433F-BEEF-AB601CF404FD}" name="Silicon" dataDxfId="41"/>
-    <tableColumn id="20" xr3:uid="{3EDDDA11-452E-44ED-90F9-73AFF8BDD363}" name="Sulfur" dataDxfId="40"/>
-    <tableColumn id="21" xr3:uid="{FF172B42-24CE-4D0F-92D0-92F16A3DF949}" name="Tellurium" dataDxfId="39"/>
-    <tableColumn id="22" xr3:uid="{975E6D5B-8CAD-42F6-BDE9-1127B7DCBFF9}" name="Titanium" dataDxfId="38"/>
-    <tableColumn id="23" xr3:uid="{F71E2C3F-5EBE-4090-BF32-6974C4A5EDCC}" name="Tungsten" dataDxfId="37"/>
-    <tableColumn id="24" xr3:uid="{01D2EA08-EA9F-4007-B864-8E90F20062F0}" name="Vanadium" dataDxfId="36"/>
-    <tableColumn id="27" xr3:uid="{705523DA-EBA3-4141-945C-D68DA3C794F1}" name="Zinc" dataDxfId="35"/>
-    <tableColumn id="25" xr3:uid="{6A5FA704-A8CD-4253-BD8C-2B56E6FDADB4}" name="Zirconium" dataDxfId="34"/>
-    <tableColumn id="29" xr3:uid="{A2AB44F8-5F8C-45E9-A300-A906A8211376}" name="Other Chemical" dataDxfId="33"/>
-    <tableColumn id="37" xr3:uid="{0B146C0D-D04E-4AAB-93D5-8630CADC2974}" name="Thickness" dataDxfId="32"/>
-    <tableColumn id="39" xr3:uid="{AC8B6894-83E7-4AA2-A8A4-41038B075899}" name="Inside Diameter" dataDxfId="31"/>
-    <tableColumn id="38" xr3:uid="{D8C783B3-2DC5-4FC0-82EA-9E6E9486B395}" name="Outside Diameter" dataDxfId="30"/>
-    <tableColumn id="36" xr3:uid="{1DCCC6B8-819E-4457-9C71-253F5BC787D5}" name="Length" dataDxfId="29"/>
-    <tableColumn id="35" xr3:uid="{3B3C6CCD-F415-4188-90FF-18A099AA63D1}" name="Width" dataDxfId="28"/>
-    <tableColumn id="34" xr3:uid="{FECE9BE4-EAE5-435F-B395-21EE384465CB}" name="Height" dataDxfId="27"/>
-    <tableColumn id="42" xr3:uid="{F9F64D39-3714-4478-BC72-D162CF1741B0}" name="Tensile Strength" dataDxfId="26"/>
-    <tableColumn id="41" xr3:uid="{D7892FB4-4842-47A4-AD5F-74F65B909CD4}" name="Yield Strength" dataDxfId="25"/>
-    <tableColumn id="40" xr3:uid="{3AD87137-2713-48AA-BCAA-014FAA2B61CD}" name="Hardness" dataDxfId="24"/>
-    <tableColumn id="44" xr3:uid="{6DF44EB3-778D-4D69-BB12-9EC2E1AC635B}" name="Elogation" dataDxfId="23"/>
-    <tableColumn id="46" xr3:uid="{C315E703-6E42-4575-BF91-DEA161BD8545}" name="Reduction in Area" dataDxfId="22"/>
-    <tableColumn id="45" xr3:uid="{DC169605-06F8-4D9B-9191-2D074DEB1C8B}" name="Hole Expansion" dataDxfId="21"/>
-    <tableColumn id="48" xr3:uid="{18F73682-85E1-4B7A-9E16-7492136AA9E4}" name="Bendability" dataDxfId="20"/>
-    <tableColumn id="49" xr3:uid="{E6103022-01BB-40A1-8E0F-A0E59220B103}" name="Epstein Test" dataDxfId="19"/>
-    <tableColumn id="51" xr3:uid="{366F8B3D-E5B7-4524-B010-0365DA18AB18}" name="Greer Lab Method" dataDxfId="18"/>
-    <tableColumn id="50" xr3:uid="{6603C2DE-C137-479B-8124-CBE8359870A0}" name="Stacked Wide Sheet" dataDxfId="17"/>
-    <tableColumn id="47" xr3:uid="{CE6518EA-E32A-490D-B8FA-C5F9E9B7206B}" name="Profilometer" dataDxfId="16"/>
+    <tableColumn id="52" xr3:uid="{AF00D49C-0A7D-4826-8506-CA4526F98C11}" name="Product Description" dataDxfId="62" dataCellStyle="Neutral"/>
+    <tableColumn id="2" xr3:uid="{A687C822-C58F-452D-B26B-CD9856126779}" name="Aluminum" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{B1E51DF4-E370-4B45-B934-CA4680543E00}" name="Antimony" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{7D4E5A00-87A1-4DB6-9285-237214866EA7}" name="Bismuth" dataDxfId="59"/>
+    <tableColumn id="5" xr3:uid="{FF6AE917-6EF7-453D-B900-491D429EA10B}" name="Boron" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{C6ABA99D-1825-4988-8F10-DA21B5E30466}" name="Carbon" dataDxfId="57"/>
+    <tableColumn id="7" xr3:uid="{91DDBD07-BA6D-41D3-9082-B8FF3D52C3E3}" name="Chromium" dataDxfId="56"/>
+    <tableColumn id="8" xr3:uid="{BA93B31C-68BB-4929-94DC-EAD966AE376B}" name="Cobalt" dataDxfId="55"/>
+    <tableColumn id="9" xr3:uid="{1FDAC7B7-2C23-4E6E-92BF-72B3374222D5}" name="Copper" dataDxfId="54"/>
+    <tableColumn id="10" xr3:uid="{27E624C3-C609-4CA7-8BE0-5CE724DAB152}" name="Iron" dataDxfId="53"/>
+    <tableColumn id="11" xr3:uid="{7DBD8888-7842-48EA-AE28-BEE69CF5DC79}" name="Lead" dataDxfId="52"/>
+    <tableColumn id="28" xr3:uid="{DF0716E0-9874-4A86-8764-FB0155320B9F}" name="Magnesium" dataDxfId="51"/>
+    <tableColumn id="12" xr3:uid="{F4F409FB-A7C8-4EB9-8DCC-EE00D05071BC}" name="Manganese" dataDxfId="50"/>
+    <tableColumn id="13" xr3:uid="{DEA2DC2F-313C-4BC9-8D50-5353297D4F05}" name="Molybdenum" dataDxfId="49"/>
+    <tableColumn id="14" xr3:uid="{43C014BD-631A-4A5B-A695-5EE01DBB3143}" name="Nickel" dataDxfId="48"/>
+    <tableColumn id="15" xr3:uid="{2D60D17D-1D84-4C39-8B26-9695D79B6202}" name="Niobium" dataDxfId="47"/>
+    <tableColumn id="16" xr3:uid="{31EFBEBA-E25A-414C-9C97-44B44C2668F7}" name="Nitrogen" dataDxfId="46"/>
+    <tableColumn id="17" xr3:uid="{67D70C10-B973-4F94-9919-EEE95AABDDE6}" name="Phosphorus" dataDxfId="45"/>
+    <tableColumn id="18" xr3:uid="{6966F273-C0D5-4B0D-B67C-96CA2143F39B}" name="Selenium" dataDxfId="44"/>
+    <tableColumn id="19" xr3:uid="{34637CE8-6F73-433F-BEEF-AB601CF404FD}" name="Silicon" dataDxfId="43"/>
+    <tableColumn id="20" xr3:uid="{3EDDDA11-452E-44ED-90F9-73AFF8BDD363}" name="Sulfur" dataDxfId="42"/>
+    <tableColumn id="21" xr3:uid="{FF172B42-24CE-4D0F-92D0-92F16A3DF949}" name="Tellurium" dataDxfId="41"/>
+    <tableColumn id="22" xr3:uid="{975E6D5B-8CAD-42F6-BDE9-1127B7DCBFF9}" name="Titanium" dataDxfId="40"/>
+    <tableColumn id="23" xr3:uid="{F71E2C3F-5EBE-4090-BF32-6974C4A5EDCC}" name="Tungsten" dataDxfId="39"/>
+    <tableColumn id="24" xr3:uid="{01D2EA08-EA9F-4007-B864-8E90F20062F0}" name="Vanadium" dataDxfId="38"/>
+    <tableColumn id="27" xr3:uid="{705523DA-EBA3-4141-945C-D68DA3C794F1}" name="Zinc" dataDxfId="37"/>
+    <tableColumn id="25" xr3:uid="{6A5FA704-A8CD-4253-BD8C-2B56E6FDADB4}" name="Zirconium" dataDxfId="36"/>
+    <tableColumn id="29" xr3:uid="{A2AB44F8-5F8C-45E9-A300-A906A8211376}" name="Other Chemical" dataDxfId="35"/>
+    <tableColumn id="37" xr3:uid="{0B146C0D-D04E-4AAB-93D5-8630CADC2974}" name="Thickness" dataDxfId="34"/>
+    <tableColumn id="39" xr3:uid="{AC8B6894-83E7-4AA2-A8A4-41038B075899}" name="Inside Diameter" dataDxfId="33"/>
+    <tableColumn id="38" xr3:uid="{D8C783B3-2DC5-4FC0-82EA-9E6E9486B395}" name="Outside Diameter" dataDxfId="32"/>
+    <tableColumn id="36" xr3:uid="{1DCCC6B8-819E-4457-9C71-253F5BC787D5}" name="Length" dataDxfId="31"/>
+    <tableColumn id="35" xr3:uid="{3B3C6CCD-F415-4188-90FF-18A099AA63D1}" name="Width" dataDxfId="30"/>
+    <tableColumn id="34" xr3:uid="{FECE9BE4-EAE5-435F-B395-21EE384465CB}" name="Height" dataDxfId="29"/>
+    <tableColumn id="42" xr3:uid="{F9F64D39-3714-4478-BC72-D162CF1741B0}" name="Tensile Strength" dataDxfId="28"/>
+    <tableColumn id="41" xr3:uid="{D7892FB4-4842-47A4-AD5F-74F65B909CD4}" name="Yield Strength" dataDxfId="27"/>
+    <tableColumn id="40" xr3:uid="{3AD87137-2713-48AA-BCAA-014FAA2B61CD}" name="Hardness" dataDxfId="26"/>
+    <tableColumn id="44" xr3:uid="{6DF44EB3-778D-4D69-BB12-9EC2E1AC635B}" name="Elogation" dataDxfId="25"/>
+    <tableColumn id="46" xr3:uid="{C315E703-6E42-4575-BF91-DEA161BD8545}" name="Reduction in Area" dataDxfId="24"/>
+    <tableColumn id="45" xr3:uid="{DC169605-06F8-4D9B-9191-2D074DEB1C8B}" name="Hole Expansion" dataDxfId="23"/>
+    <tableColumn id="48" xr3:uid="{18F73682-85E1-4B7A-9E16-7492136AA9E4}" name="Bendability" dataDxfId="22"/>
+    <tableColumn id="49" xr3:uid="{E6103022-01BB-40A1-8E0F-A0E59220B103}" name="Epstein Test" dataDxfId="21"/>
+    <tableColumn id="51" xr3:uid="{366F8B3D-E5B7-4524-B010-0365DA18AB18}" name="Greer Lab Method" dataDxfId="20"/>
+    <tableColumn id="50" xr3:uid="{6603C2DE-C137-479B-8124-CBE8359870A0}" name="Stacked Wide Sheet" dataDxfId="19"/>
+    <tableColumn id="47" xr3:uid="{CE6518EA-E32A-490D-B8FA-C5F9E9B7206B}" name="Profilometer" dataDxfId="18"/>
     <tableColumn id="26" xr3:uid="{954B900D-2AB0-4B19-9176-3C7B61D42BBB}" name="Active"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2877,13 +2895,15 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{650EAF1A-DBF8-457D-8987-08024C2AC249}" name="Table2" displayName="Table2" ref="B1:F5" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="B1:F5" xr:uid="{83E92AFF-20AE-48D4-A5DC-3FC33C56D7BA}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{329825AA-46A8-456B-B9C3-77BB28B256F9}" name="Application Suitability" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{B091EF3F-84F5-4061-BA8E-33B723663C19}" name="Origin Country" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{4C9E8D40-0D96-4F2B-8835-53C450182880}" name="Export Country" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{38EC2BA1-0435-4A0F-A69B-27868857F181}" name="CBP Distinguish Comments" dataDxfId="11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{650EAF1A-DBF8-457D-8987-08024C2AC249}" name="Table2" displayName="Table2" ref="B1:H6" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="B1:H6" xr:uid="{83E92AFF-20AE-48D4-A5DC-3FC33C56D7BA}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{329825AA-46A8-456B-B9C3-77BB28B256F9}" name="Application Suitability" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{B091EF3F-84F5-4061-BA8E-33B723663C19}" name="Origin Country" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{4C9E8D40-0D96-4F2B-8835-53C450182880}" name="Export Country" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{4D9B8641-A284-448A-B88A-0CBC38A63AF5}" name="Exclusion Quantity" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{38EC2BA1-0435-4A0F-A69B-27868857F181}" name="CBP Distinguish Comments" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{D7B89058-93A1-4C84-8D98-982362B8E521}" name="Column1" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{01FA5224-A264-4AE2-A1E8-578EA0346DD6}" name="Active" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2891,8 +2911,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7FCBF9CA-1F8C-4B37-8C0F-9331F9CFCC5D}" name="Table3" displayName="Table3" ref="B1:I5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowCellStyle="Neutral" dataCellStyle="Neutral">
-  <autoFilter ref="B1:I5" xr:uid="{F5EEA5D1-B24E-43E7-B766-62B39E18849A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7FCBF9CA-1F8C-4B37-8C0F-9331F9CFCC5D}" name="Table3" displayName="Table3" ref="B1:I6" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowCellStyle="Neutral" dataCellStyle="Neutral">
+  <autoFilter ref="B1:I6" xr:uid="{F5EEA5D1-B24E-43E7-B766-62B39E18849A}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7A6A68FC-6E83-4B7E-BAC2-C8A0BF1DECBE}" name="Submission Certification Authorizing Official Company Name" dataDxfId="7" dataCellStyle="Neutral"/>
     <tableColumn id="2" xr3:uid="{BD1154E5-D376-4BA8-AC9D-24A249216F1A}" name="Submission Certification Authorizing Official Name" dataDxfId="6" dataCellStyle="Neutral"/>
@@ -3172,8 +3192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6561DE94-E3AB-4C26-84CE-440BF0BDEA94}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3194,7 +3214,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3202,7 +3222,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -3218,12 +3238,12 @@
         <v>30</v>
       </c>
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -3244,10 +3264,10 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q8" sqref="Q8"/>
+      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3281,67 +3301,67 @@
         <v>26</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E1" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="M1" s="16" t="s">
+        <v>446</v>
+      </c>
+      <c r="N1" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="O1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="R1" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="S1" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="M1" s="16" t="s">
-        <v>450</v>
-      </c>
-      <c r="N1" s="16" t="s">
+      <c r="T1" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="U1" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="O1" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="R1" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="S1" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="T1" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="U1" s="16" t="s">
-        <v>130</v>
-      </c>
       <c r="V1" s="16" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="W1" s="16" t="s">
         <v>0</v>
@@ -3352,23 +3372,25 @@
         <v>27</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>562</v>
+        <v>573</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="F2" s="20"/>
+        <v>115</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>574</v>
+      </c>
       <c r="G2" s="20" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I2" s="20">
         <v>555</v>
@@ -3380,35 +3402,37 @@
         <v>58455555</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>139</v>
+        <v>137</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>459</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="O2" s="20"/>
+        <v>115</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>435</v>
+      </c>
       <c r="P2" s="20" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="Q2" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R2" s="20" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="S2" s="20" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="U2" s="20" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="V2" s="20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="W2" s="20" t="b">
         <v>0</v>
@@ -3419,52 +3443,54 @@
         <v>28</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="C3" s="20" t="s">
-        <v>189</v>
-      </c>
       <c r="D3" s="20" t="s">
-        <v>563</v>
-      </c>
-      <c r="E3" s="20"/>
+        <v>573</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>115</v>
+      </c>
       <c r="F3" s="20" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="G3" s="20">
         <v>33333</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
       <c r="L3" s="20"/>
       <c r="M3" s="16" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="N3" s="20"/>
       <c r="O3" s="20" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="P3" s="20" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="Q3" s="20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
       <c r="T3" s="20"/>
       <c r="U3" s="20"/>
       <c r="V3" s="16" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="W3" s="20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -3472,49 +3498,51 @@
         <v>29</v>
       </c>
       <c r="B4" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>189</v>
-      </c>
       <c r="D4" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="E4" s="20"/>
+        <v>573</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>115</v>
+      </c>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
       <c r="K4" s="20" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="N4" s="20"/>
       <c r="O4" s="20"/>
       <c r="P4" s="20"/>
       <c r="Q4" s="20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="R4" s="20" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="S4" s="20"/>
       <c r="T4" s="20" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="U4" s="20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="V4" s="16" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="W4" s="20" t="b">
         <v>0</v>
@@ -3525,134 +3553,138 @@
         <v>30</v>
       </c>
       <c r="B5" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="D5" s="20"/>
+      <c r="D5" s="20" t="s">
+        <v>573</v>
+      </c>
       <c r="E5" s="20" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F5" s="20" t="s">
+        <v>453</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>454</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>455</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>456</v>
+      </c>
+      <c r="K5" s="20" t="s">
         <v>457</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="L5" s="16" t="s">
         <v>458</v>
       </c>
-      <c r="H5" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="I5" s="20" t="s">
+      <c r="M5" s="16" t="s">
         <v>459</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="N5" s="20" t="s">
+        <v>465</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>464</v>
+      </c>
+      <c r="P5" s="20" t="s">
+        <v>463</v>
+      </c>
+      <c r="Q5" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="R5" s="20" t="s">
+        <v>455</v>
+      </c>
+      <c r="S5" s="20" t="s">
+        <v>461</v>
+      </c>
+      <c r="T5" s="20" t="s">
+        <v>462</v>
+      </c>
+      <c r="U5" s="16" t="s">
+        <v>458</v>
+      </c>
+      <c r="V5" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="K5" s="20" t="s">
-        <v>461</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>462</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>463</v>
-      </c>
-      <c r="N5" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="O5" s="20" t="s">
-        <v>468</v>
-      </c>
-      <c r="P5" s="20" t="s">
-        <v>467</v>
-      </c>
-      <c r="Q5" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="R5" s="20" t="s">
-        <v>459</v>
-      </c>
-      <c r="S5" s="20" t="s">
-        <v>465</v>
-      </c>
-      <c r="T5" s="20" t="s">
-        <v>466</v>
-      </c>
-      <c r="U5" s="16" t="s">
-        <v>462</v>
-      </c>
-      <c r="V5" s="16" t="s">
-        <v>464</v>
-      </c>
       <c r="W5" s="20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="D6" s="20"/>
+        <v>197</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>573</v>
+      </c>
       <c r="E6" s="20" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="G6" s="20" t="s">
+        <v>454</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>559</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>456</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>457</v>
+      </c>
+      <c r="L6" s="16" t="s">
         <v>458</v>
       </c>
-      <c r="H6" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>565</v>
-      </c>
-      <c r="J6" s="20" t="s">
+      <c r="M6" s="16" t="s">
+        <v>459</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>560</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>464</v>
+      </c>
+      <c r="P6" s="20" t="s">
+        <v>463</v>
+      </c>
+      <c r="Q6" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="R6" s="20" t="s">
+        <v>559</v>
+      </c>
+      <c r="S6" s="20" t="s">
+        <v>561</v>
+      </c>
+      <c r="T6" s="20" t="s">
+        <v>462</v>
+      </c>
+      <c r="U6" s="16" t="s">
+        <v>458</v>
+      </c>
+      <c r="V6" s="16" t="s">
         <v>460</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>461</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>462</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>463</v>
-      </c>
-      <c r="N6" s="20" t="s">
-        <v>566</v>
-      </c>
-      <c r="O6" s="20" t="s">
-        <v>468</v>
-      </c>
-      <c r="P6" s="20" t="s">
-        <v>467</v>
-      </c>
-      <c r="Q6" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="R6" s="20" t="s">
-        <v>565</v>
-      </c>
-      <c r="S6" s="20" t="s">
-        <v>567</v>
-      </c>
-      <c r="T6" s="20" t="s">
-        <v>466</v>
-      </c>
-      <c r="U6" s="16" t="s">
-        <v>462</v>
-      </c>
-      <c r="V6" s="16" t="s">
-        <v>464</v>
       </c>
       <c r="W6" s="20" t="b">
         <v>0</v>
@@ -3689,13 +3721,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDF6C06-83F3-41E7-8AF0-9CE3125477FE}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R3" sqref="R3"/>
+      <selection pane="bottomRight" activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3724,52 +3756,52 @@
         <v>26</v>
       </c>
       <c r="B1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" t="s">
+        <v>442</v>
+      </c>
+      <c r="E1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" t="s">
         <v>211</v>
       </c>
-      <c r="C1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D1" t="s">
-        <v>446</v>
-      </c>
-      <c r="E1" t="s">
-        <v>213</v>
-      </c>
-      <c r="F1" t="s">
-        <v>214</v>
-      </c>
-      <c r="G1" t="s">
-        <v>215</v>
-      </c>
       <c r="H1" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="I1" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="J1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="K1" t="s">
+        <v>424</v>
+      </c>
+      <c r="L1" t="s">
+        <v>425</v>
+      </c>
+      <c r="M1" t="s">
+        <v>426</v>
+      </c>
+      <c r="N1" t="s">
+        <v>427</v>
+      </c>
+      <c r="O1" t="s">
         <v>428</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>429</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>430</v>
-      </c>
-      <c r="N1" t="s">
-        <v>431</v>
-      </c>
-      <c r="O1" t="s">
-        <v>432</v>
-      </c>
-      <c r="P1" t="s">
-        <v>433</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>434</v>
       </c>
       <c r="R1" t="s">
         <v>0</v>
@@ -3780,55 +3812,55 @@
         <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>433</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>443</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>437</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>447</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="L2" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>444</v>
-      </c>
       <c r="Q2" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="R2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -3836,48 +3868,48 @@
         <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>445</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="R3" t="b">
         <v>0</v>
@@ -3888,49 +3920,49 @@
         <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="R4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -3938,69 +3970,125 @@
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>468</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="I5" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="J5" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="O5" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>480</v>
-      </c>
       <c r="Q5" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="R5" t="b">
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>468</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="R6" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5" xr:uid="{579BED46-8514-4FBB-A799-15A182FB28BF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6" xr:uid="{579BED46-8514-4FBB-A799-15A182FB28BF}">
       <formula1>activity</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5 Q2:Q5" xr:uid="{BF845D3C-B3D9-4135-B581-87B72DE837CD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6 Q2:Q6" xr:uid="{BF845D3C-B3D9-4135-B581-87B72DE837CD}">
       <formula1>country</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J5" xr:uid="{CFA3E274-170C-4C85-AFBE-A694C971741C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J6" xr:uid="{CFA3E274-170C-4C85-AFBE-A694C971741C}">
       <formula1>exclusive_expl</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R5" xr:uid="{1FED2DD3-AB26-4661-8ECB-A5A59A5A0B76}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R6" xr:uid="{1FED2DD3-AB26-4661-8ECB-A5A59A5A0B76}">
       <formula1>tf</formula1>
     </dataValidation>
   </dataValidations>
@@ -4014,13 +4102,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU5"/>
+  <dimension ref="A1:AU6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AJ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AU3" sqref="AU3:AU5"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4057,7 +4145,7 @@
         <v>26</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -4141,55 +4229,55 @@
         <v>33</v>
       </c>
       <c r="AD1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG1" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AH1" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AI1" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="AG1" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="AH1" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="AI1" s="12" t="s">
+      <c r="AJ1" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="AK1" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="AJ1" s="13" t="s">
+      <c r="AL1" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="AM1" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="AN1" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="AO1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="AK1" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="AL1" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="AM1" s="15" t="s">
+      <c r="AP1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="AN1" s="15" t="s">
+      <c r="AQ1" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="AO1" s="15" t="s">
+      <c r="AR1" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="AP1" s="15" t="s">
+      <c r="AS1" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="AQ1" s="14" t="s">
+      <c r="AT1" s="14" t="s">
         <v>104</v>
-      </c>
-      <c r="AR1" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="AS1" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="AT1" s="14" t="s">
-        <v>107</v>
       </c>
       <c r="AU1" s="7" t="s">
         <v>0</v>
@@ -4200,31 +4288,31 @@
         <v>27</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>78</v>
+        <v>569</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>87</v>
+        <v>570</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>41</v>
@@ -4233,10 +4321,10 @@
         <v>38</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>42</v>
@@ -4296,19 +4384,19 @@
         <v>55</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AJ2" s="1" t="s">
         <v>54</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="AM2" s="1" t="s">
         <v>52</v>
@@ -4317,25 +4405,25 @@
         <v>53</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AU2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.3">
@@ -4344,16 +4432,16 @@
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>57</v>
@@ -4440,7 +4528,7 @@
         <v>74</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AJ3" s="1" t="s">
         <v>53</v>
@@ -4467,13 +4555,13 @@
         <v>74</v>
       </c>
       <c r="AR3" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AS3" s="1" t="s">
         <v>74</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AU3" t="b">
         <v>0</v>
@@ -4485,136 +4573,136 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="K4" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>497</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>39</v>
       </c>
       <c r="R4" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="AC4" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="AE4" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AG4" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AM4" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="AB4" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AN4" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="AD4" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AO4" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AR4" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="AG4" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="AH4" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="AI4" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="AJ4" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="AK4" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="AL4" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="AM4" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="AN4" s="1" t="s">
+      <c r="AS4" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="AT4" s="1" t="s">
         <v>512</v>
-      </c>
-      <c r="AO4" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="AP4" s="1" t="s">
-        <v>528</v>
-      </c>
-      <c r="AQ4" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="AR4" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="AS4" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="AT4" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="AU4" t="b">
         <v>0</v>
@@ -4625,7 +4713,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>34</v>
@@ -4640,16 +4728,16 @@
         <v>36</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>75</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>76</v>
@@ -4667,7 +4755,7 @@
         <v>36</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>35</v>
@@ -4676,7 +4764,7 @@
         <v>75</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>76</v>
@@ -4694,7 +4782,7 @@
         <v>36</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="Z5" s="1" t="s">
         <v>35</v>
@@ -4703,7 +4791,7 @@
         <v>75</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="AC5" s="1" t="s">
         <v>76</v>
@@ -4721,7 +4809,7 @@
         <v>36</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="AI5" s="1" t="s">
         <v>35</v>
@@ -4730,7 +4818,7 @@
         <v>75</v>
       </c>
       <c r="AK5" s="1" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="AL5" s="1" t="s">
         <v>76</v>
@@ -4748,7 +4836,7 @@
         <v>36</v>
       </c>
       <c r="AQ5" s="1" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="AR5" s="1" t="s">
         <v>35</v>
@@ -4757,9 +4845,152 @@
         <v>75</v>
       </c>
       <c r="AT5" s="1" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="AU5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ6" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="AR6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AS6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT6" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="AU6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4774,7 +5005,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1" xr:uid="{BC057764-74F1-455D-8290-8135998C00FF}">
       <formula1>state</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2:AU5" xr:uid="{CD1C6A87-9A17-4A73-BA1D-5F8FA8210BB6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2:AU6" xr:uid="{CD1C6A87-9A17-4A73-BA1D-5F8FA8210BB6}">
       <formula1>tf</formula1>
     </dataValidation>
   </dataValidations>
@@ -4791,13 +5022,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2B0A54-C8B7-4DE9-83A1-D8B079339484}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4805,106 +5036,152 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.21875" customWidth="1"/>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="4" max="5" width="15.5546875" customWidth="1"/>
+    <col min="6" max="7" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>454</v>
-      </c>
-      <c r="F1" s="19" t="s">
+        <v>576</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>450</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>575</v>
+      </c>
+      <c r="H1" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="b">
+        <v>134</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="b">
+        <v>218</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="F5" s="1" t="b">
+        <v>578</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D5" xr:uid="{48B472F1-1596-4C16-901B-59906CFA2FD7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D6" xr:uid="{48B472F1-1596-4C16-901B-59906CFA2FD7}">
       <formula1>country</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5" xr:uid="{520C7828-6067-4DB6-B570-B75272DBA74B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H6" xr:uid="{520C7828-6067-4DB6-B570-B75272DBA74B}">
       <formula1>tf</formula1>
     </dataValidation>
   </dataValidations>
@@ -4920,11 +5197,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E335BF1-D685-43ED-A123-7112467278F5}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4944,25 +5221,25 @@
         <v>26</v>
       </c>
       <c r="B1" s="25" t="s">
+        <v>525</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>526</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>527</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>528</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="G1" s="25" t="s">
         <v>530</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="H1" s="25" t="s">
         <v>531</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>532</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>533</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>534</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>535</v>
       </c>
       <c r="I1" s="19" t="s">
         <v>0</v>
@@ -4988,25 +5265,25 @@
         <v>28</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="I3" s="22" t="b">
         <v>0</v>
@@ -5020,16 +5297,16 @@
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
       <c r="E4" s="24" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="I4" s="22" t="b">
         <v>0</v>
@@ -5040,38 +5317,62 @@
         <v>30</v>
       </c>
       <c r="B5" s="21" t="s">
+        <v>532</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>533</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>534</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>537</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>535</v>
+      </c>
+      <c r="G5" s="23" t="s">
         <v>536</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="H5" s="21" t="s">
         <v>537</v>
       </c>
-      <c r="D5" s="21" t="s">
-        <v>538</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>541</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>539</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>540</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>541</v>
-      </c>
       <c r="I5" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>561</v>
+        <v>557</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>532</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>533</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>534</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>537</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>535</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>536</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>537</v>
+      </c>
+      <c r="I6" s="22" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I5" xr:uid="{EB551C7A-8C81-46A2-9AE5-3F7FA6B6C498}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6" xr:uid="{EB551C7A-8C81-46A2-9AE5-3F7FA6B6C498}">
       <formula1>tf</formula1>
     </dataValidation>
   </dataValidations>
@@ -5088,7 +5389,7 @@
   <dimension ref="A1:H201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5119,250 +5420,250 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B1" t="b">
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G2" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="H2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="F3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G3" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="H3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="G4" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="H4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="H5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G6" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="H6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H8" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H13" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H14" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H15" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H16" t="s">
         <v>1</v>
@@ -5370,1035 +5671,1035 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="16" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="16" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="16" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="16" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="16" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="16" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="16" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="16" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="16" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="16" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="16" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="16" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="16" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="16" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="16" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="16" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="16" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="16" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="16" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="16" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="16" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="16" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="16" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="16" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="16" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="16" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="16" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="16" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="16" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="16" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="16" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="16" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="16" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="16" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="16" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="16" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="16" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="16" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="16" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="16" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="16" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="16" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="16" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="16" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="16" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="16" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="16" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="16" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="16" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="16" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" s="16" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="16" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="16" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="16" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="16" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="16" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="16" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="16" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="16" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="16" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="16" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="16" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="16" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="16" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="16" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="16" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="16" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="16" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="16" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="16" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="16" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="16" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="16" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="16" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="16" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="16" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="16" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="16" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="16" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="16" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="16" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="16" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="16" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="16" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="16" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="16" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="16" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="16" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="16" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="16" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="16" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="16" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" s="16" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="16" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" s="16" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" s="16" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" s="16" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="16" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="16" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" s="16" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="16" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" s="16" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="16" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="16" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" s="16" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" s="16" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" s="16" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" s="16" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" s="16" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" s="16" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" s="16" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" s="16" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" s="16" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" s="16" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="16" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="16" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" s="16" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" s="16" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" s="16" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" s="16" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" s="16" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" s="16" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" s="16" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" s="16" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" s="16" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" s="16" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" s="16" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" s="16" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" s="16" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" s="16" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" s="16" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" s="16" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" s="16" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" s="16" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" s="16" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" s="16" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" s="16" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" s="16" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" s="16" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="16" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="16" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" s="16" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" s="16" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" s="16" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" s="16" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="16" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" s="16" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" s="16" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" s="16" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" s="16" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" s="16" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" s="16" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" s="16" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200" s="16" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" s="16" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>